<commit_message>
Changed skill id to be an enum instead of string
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755D9FCB-24BC-4E27-ABD1-1061C757D581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B11EBB1-4B99-4960-B3EB-60313B7F0299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="870" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>枚举名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>SkillId</t>
+  </si>
+  <si>
+    <t>CHAIN_LIGHTNING</t>
+  </si>
+  <si>
+    <t>EXPLOSION</t>
+  </si>
+  <si>
+    <t>SLOW</t>
   </si>
 </sst>
 </file>
@@ -519,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482160D1-8E9F-4701-8C89-55D43E73138E}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -676,6 +688,47 @@
         <v>5</v>
       </c>
     </row>
+    <row r="10" spans="1:11">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:K1"/>

</xml_diff>

<commit_message>
Added SkillType enum in configs
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815929CC-8C0F-41F5-9EDE-FE9D50C06BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB2B447-255D-4FBA-96EC-3BCE2EABEBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="870" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
+    <workbookView xWindow="4080" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>枚举名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>SLOW</t>
+  </si>
+  <si>
+    <t>SkillType</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>PASSIVE</t>
   </si>
 </sst>
 </file>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482160D1-8E9F-4701-8C89-55D43E73138E}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -729,6 +738,31 @@
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="1:11">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:K1"/>

</xml_diff>

<commit_message>
Add passive skill ATTACK
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB2B447-255D-4FBA-96EC-3BCE2EABEBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E020E44F-CB5D-414D-BFB1-993F8F838EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>枚举名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482160D1-8E9F-4701-8C89-55D43E73138E}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -739,27 +739,35 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="B14" t="s">
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="b">
+      <c r="C15" t="b">
         <v>0</v>
       </c>
-      <c r="D14" t="b">
+      <c r="D15" t="b">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>32</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="G15" t="s">
+    <row r="16" spans="1:11">
+      <c r="G16" t="s">
         <v>33</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add SkillAttributeManager to manage both common and specific skill attributes
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E020E44F-CB5D-414D-BFB1-993F8F838EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0D59FA-2B02-42B4-9CB0-C6F190D6CF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="3645" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
+    <workbookView xWindow="3735" yWindow="3300" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>枚举名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,9 +137,6 @@
     <t>EXPLOSION</t>
   </si>
   <si>
-    <t>SLOW</t>
-  </si>
-  <si>
     <t>SkillType</t>
   </si>
   <si>
@@ -147,6 +144,15 @@
   </si>
   <si>
     <t>PASSIVE</t>
+  </si>
+  <si>
+    <t>COMMON</t>
+  </si>
+  <si>
+    <t>ONE_PUNCH</t>
+  </si>
+  <si>
+    <t>SHOCK_WAVE</t>
   </si>
 </sst>
 </file>
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482160D1-8E9F-4701-8C89-55D43E73138E}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -708,7 +714,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -732,7 +738,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="G13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I13">
         <v>3</v>
@@ -740,34 +746,42 @@
     </row>
     <row r="14" spans="1:11">
       <c r="G14" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="I14">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="B15" t="s">
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="b">
+      <c r="I16">
         <v>0</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
+    </row>
+    <row r="17" spans="7:9">
+      <c r="G17" t="s">
         <v>32</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16">
+      <c r="I17">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made level as a skill attribute
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0D59FA-2B02-42B4-9CB0-C6F190D6CF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2227CF30-E7B2-47DF-A210-8318CBB435CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="3300" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
   </bookViews>
@@ -125,9 +125,6 @@
     <t>ATTACK_DECREASE</t>
   </si>
   <si>
-    <t>NONE</t>
-  </si>
-  <si>
     <t>SkillId</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>SHOCK_WAVE</t>
+  </si>
+  <si>
+    <t>LEVEL</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -714,7 +714,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="G11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="G12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="G13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13">
         <v>3</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="G14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I14">
         <v>4</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="17" spans="7:9">
       <c r="G17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17">
         <v>1</v>

</xml_diff>

<commit_message>
Added new attribute types: CD, SPEED, PIERCE
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tigersun/Code/GobangAdventure/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695A1BEC-0DE0-48A2-802B-C49B30AE0D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A324B01D-90DB-C643-A3C3-C78259BBBBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9885" yWindow="4590" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>枚举名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -156,13 +156,22 @@
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>SPEED</t>
+  </si>
+  <si>
+    <t>PIERCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,7 +550,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,26 +558,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482160D1-8E9F-4701-8C89-55D43E73138E}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -595,7 +604,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -620,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="99" customHeight="1">
+    <row r="3" spans="1:11" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -649,7 +658,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -666,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G5" t="s">
         <v>35</v>
       </c>
@@ -674,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G6" t="s">
         <v>21</v>
       </c>
@@ -682,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G7" t="s">
         <v>22</v>
       </c>
@@ -690,7 +699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G8" t="s">
         <v>23</v>
       </c>
@@ -698,7 +707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G9" t="s">
         <v>24</v>
       </c>
@@ -706,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
         <v>25</v>
       </c>
@@ -714,85 +723,109 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="B11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="b">
+      <c r="C14" t="b">
         <v>0</v>
       </c>
-      <c r="D11" t="b">
+      <c r="D14" t="b">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G14" t="s">
         <v>32</v>
       </c>
-      <c r="I11">
+      <c r="I14">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="G12" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
         <v>27</v>
       </c>
-      <c r="I12">
+      <c r="I15">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="G13" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
         <v>28</v>
       </c>
-      <c r="I13">
+      <c r="I16">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="G14" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
         <v>33</v>
       </c>
-      <c r="I14">
+      <c r="I17">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="G15" t="s">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
         <v>34</v>
       </c>
-      <c r="I15">
+      <c r="I18">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="G16" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
         <v>21</v>
       </c>
-      <c r="I16">
+      <c r="I19">
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
-      <c r="B17" t="s">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="b">
+      <c r="C20" t="b">
         <v>0</v>
       </c>
-      <c r="D17" t="b">
+      <c r="D20" t="b">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G20" t="s">
         <v>30</v>
       </c>
-      <c r="I17">
+      <c r="I20">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
-      <c r="G18" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
         <v>31</v>
       </c>
-      <c r="I18">
+      <c r="I21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make SkillBehaviorType as one of the attribute instead of a field in skill config
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tigersun/Code/GobangAdventure/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A324B01D-90DB-C643-A3C3-C78259BBBBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15985458-1970-504C-831F-76459FC1E283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>枚举名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>PIERCE</t>
+  </si>
+  <si>
+    <t>BEHAVIOR_TYPE</t>
   </si>
 </sst>
 </file>
@@ -558,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482160D1-8E9F-4701-8C89-55D43E73138E}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -685,7 +688,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G6" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="I6">
         <v>2</v>
@@ -693,139 +696,147 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G11" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
         <v>39</v>
       </c>
-      <c r="I13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="I14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="b">
+      <c r="C15" t="b">
         <v>0</v>
       </c>
-      <c r="D14" t="b">
+      <c r="D15" t="b">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>32</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
         <v>21</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="C20" t="b">
+      <c r="C21" t="b">
         <v>0</v>
       </c>
-      <c r="D20" t="b">
+      <c r="D21" t="b">
         <v>1</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>30</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G21" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
         <v>31</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add skill Tian Shan Liu Yang Zhang
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__enums__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF77B97-A2FE-4035-A329-4D0157790F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F6331C-6AEB-4963-A1F7-6405A677FA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="3240" windowWidth="28800" windowHeight="15435" xr2:uid="{AEF47366-C0EE-4DD8-9053-59035C5D2322}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>枚举名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>LUO_HAN_QUAN</t>
+  </si>
+  <si>
+    <t>TIAN_SHAN_LIU_YANG_ZHANG</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482160D1-8E9F-4701-8C89-55D43E73138E}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -831,34 +834,42 @@
     </row>
     <row r="21" spans="2:9">
       <c r="G21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="G22" t="s">
         <v>21</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
-      <c r="B22" t="s">
+    <row r="23" spans="2:9">
+      <c r="B23" t="s">
         <v>29</v>
       </c>
-      <c r="C22" t="b">
+      <c r="C23" t="b">
         <v>0</v>
       </c>
-      <c r="D22" t="b">
+      <c r="D23" t="b">
         <v>1</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>30</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
-      <c r="G23" t="s">
+    <row r="24" spans="2:9">
+      <c r="G24" t="s">
         <v>31</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <v>1</v>
       </c>
     </row>

</xml_diff>